<commit_message>
Cambios menores en app.py
</commit_message>
<xml_diff>
--- a/data/Evento_2/EED.xlsx
+++ b/data/Evento_2/EED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSAENZ\Documents\Actividades CCC 2025\Festivandas 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juank\turismo-religioso-analisis\data\Evento_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F1EBBB5-D800-4DEC-8AAD-E77D847AE28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2C9CC4-C8BD-4F28-804A-7C76D4F00E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AEBBB0A-4FED-4546-B4AD-6FFBA3C6826A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7AEBBB0A-4FED-4546-B4AD-6FFBA3C6826A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja4" sheetId="1" r:id="rId1"/>

</xml_diff>